<commit_message>
API key in config file
</commit_message>
<xml_diff>
--- a/Data/Output/CandidateData.xlsx
+++ b/Data/Output/CandidateData.xlsx
@@ -742,6 +742,140 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="A10" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:8">
+      <x:c r="A15" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:8">
+      <x:c r="A16" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>